<commit_message>
implementação de testes até quinto cenário
</commit_message>
<xml_diff>
--- a/Aventura_se/src/main/resources/evidencia1.xlsx
+++ b/Aventura_se/src/main/resources/evidencia1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\programa_aventura_se\Aventura_se\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A53876A-635C-4D5B-AC91-566646302E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2831A2AB-8705-40E1-BA49-954BEF53DF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D2B04BA2-52AC-4279-83FE-A3D4B108EC90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>amazonclientevip@yahoo.com</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Identificação</t>
   </si>
   <si>
-    <t>Senha</t>
-  </si>
-  <si>
     <t>bicicleta aro 29</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>ID_006</t>
   </si>
   <si>
-    <t>Entrada</t>
-  </si>
-  <si>
-    <t>textox</t>
-  </si>
-  <si>
     <t>ID_002</t>
   </si>
   <si>
@@ -102,6 +93,60 @@
   </si>
   <si>
     <t>ID_015</t>
+  </si>
+  <si>
+    <t>frigideira</t>
+  </si>
+  <si>
+    <t>copo</t>
+  </si>
+  <si>
+    <t>console games lançamentos</t>
+  </si>
+  <si>
+    <t>fogão”</t>
+  </si>
+  <si>
+    <t>geladeira</t>
+  </si>
+  <si>
+    <t>garrafa</t>
+  </si>
+  <si>
+    <t>televisão”</t>
+  </si>
+  <si>
+    <t>clica1</t>
+  </si>
+  <si>
+    <t>clica2</t>
+  </si>
+  <si>
+    <t>clica3</t>
+  </si>
+  <si>
+    <t>clica4</t>
+  </si>
+  <si>
+    <t>clica5</t>
+  </si>
+  <si>
+    <t>clica6</t>
+  </si>
+  <si>
+    <t>Parametro 01</t>
+  </si>
+  <si>
+    <t>Parametro 02</t>
+  </si>
+  <si>
+    <t>DevBrito</t>
+  </si>
+  <si>
+    <t>0000000</t>
+  </si>
+  <si>
+    <t>06010067</t>
   </si>
 </sst>
 </file>
@@ -123,23 +168,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -147,11 +197,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,7 +225,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +557,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,18 +571,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2"/>
       <c r="E1" s="3"/>
       <c r="O1"/>
       <c r="Q1"/>
@@ -513,136 +588,173 @@
       <c r="U1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[  implementação de testes até oitavo cenário
</commit_message>
<xml_diff>
--- a/Aventura_se/src/main/resources/evidencia1.xlsx
+++ b/Aventura_se/src/main/resources/evidencia1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\programa_aventura_se\Aventura_se\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2831A2AB-8705-40E1-BA49-954BEF53DF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291175A8-6188-4365-9F7B-91DD09C01ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D2B04BA2-52AC-4279-83FE-A3D4B108EC90}"/>
   </bookViews>
@@ -104,24 +104,15 @@
     <t>console games lançamentos</t>
   </si>
   <si>
-    <t>fogão”</t>
-  </si>
-  <si>
     <t>geladeira</t>
   </si>
   <si>
     <t>garrafa</t>
   </si>
   <si>
-    <t>televisão”</t>
-  </si>
-  <si>
     <t>clica1</t>
   </si>
   <si>
-    <t>clica2</t>
-  </si>
-  <si>
     <t>clica3</t>
   </si>
   <si>
@@ -143,17 +134,26 @@
     <t>DevBrito</t>
   </si>
   <si>
-    <t>0000000</t>
-  </si>
-  <si>
     <t>06010067</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>fogão</t>
+  </si>
+  <si>
+    <t>televisão</t>
+  </si>
+  <si>
+    <t>console games lançamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -216,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,10 +242,16 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -554,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747B454C-A0C9-4D6A-8824-3DCAE4475126}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +589,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
@@ -588,7 +602,7 @@
       <c r="U1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -601,160 +615,166 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>36</v>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>35</v>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5"/>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="5"/>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5"/>
+      <c r="B13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="5"/>
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>